<commit_message>
Add tests for SetExcelWorksheetViewProperties to handle multiple worksheets.
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/SetExcelWorksheetViewProperties/Data/Definitions.xlsx
+++ b/test/regression/commands/general/SetExcelWorksheetViewProperties/Data/Definitions.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevRiv\TSTool_SourceBuild\TSTool\test\regression\commands\general\WriteTableToExcel\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\owf-gitrepos\cdss-app-tstool-test\test\regression\commands\general\SetExcelWorksheetViewProperties\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19620" windowHeight="9075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19620" windowHeight="9072"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ProjectTypes" sheetId="1" r:id="rId1"/>
+    <sheet name="Basins" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>These data are used to provide drop-down choices in the main data sheet.  Please do not edit.</t>
   </si>
@@ -135,6 +136,66 @@
   </si>
   <si>
     <t>?? Is this for flush flow? How different from Environmental Flow?</t>
+  </si>
+  <si>
+    <t>The information is taken from the BNDSS "Basin" database table.  A blank choice is OK.</t>
+  </si>
+  <si>
+    <t>Basin</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Gunnison</t>
+  </si>
+  <si>
+    <t>Metro</t>
+  </si>
+  <si>
+    <t>North Platte</t>
+  </si>
+  <si>
+    <t>Rio Grande</t>
+  </si>
+  <si>
+    <t>South Platte</t>
+  </si>
+  <si>
+    <t>Southwest</t>
+  </si>
+  <si>
+    <t>Arkansas River - Division 2</t>
+  </si>
+  <si>
+    <t>Upper Colorado River - Division 5</t>
+  </si>
+  <si>
+    <t>Gunnison River - Division 4</t>
+  </si>
+  <si>
+    <t>Metro Basin - part of Division 1</t>
+  </si>
+  <si>
+    <t>North Platte Basin - part of Division 1</t>
+  </si>
+  <si>
+    <t>Rio Grande River Basin - Division 3</t>
+  </si>
+  <si>
+    <t>South Platte Basin - Division 1</t>
+  </si>
+  <si>
+    <t>Southwest Basin - Division 7</t>
+  </si>
+  <si>
+    <t>Yampa/White</t>
+  </si>
+  <si>
+    <t>Yampa/White Basin - Division 6</t>
   </si>
 </sst>
 </file>
@@ -185,12 +246,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,36 +533,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
-    <col min="4" max="4" width="65.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="65.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -514,115 +576,225 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="92.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>